<commit_message>
Změna názvu sloupce na Nasazení pro kompatibilitu s kódem
</commit_message>
<xml_diff>
--- a/prihlaseni_hraci_test.xlsx
+++ b/prihlaseni_hraci_test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dan\Documents\DAN\ČVUT\OOP\semestralka\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81EB2A37-16EF-479F-8117-0364E3F19267}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F20F31B-CD5B-49D2-90FB-D2F77AD64AA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6C8EE765-406C-40AB-A193-14855FF8056C}"/>
   </bookViews>
@@ -50,9 +50,6 @@
     <t>Klub</t>
   </si>
   <si>
-    <t>Nasazení dle žebříčku</t>
-  </si>
-  <si>
     <t>Gender</t>
   </si>
   <si>
@@ -321,6 +318,9 @@
   </si>
   <si>
     <t>Žena</t>
+  </si>
+  <si>
+    <t>Nasazení</t>
   </si>
 </sst>
 </file>
@@ -725,7 +725,7 @@
   <dimension ref="A1:G45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -750,29 +750,29 @@
         <v>2</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>4</v>
+        <v>94</v>
       </c>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E3">
         <v>26</v>
@@ -780,16 +780,16 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
         <v>10</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" t="s">
-        <v>11</v>
       </c>
       <c r="E4">
         <v>25</v>
@@ -797,16 +797,16 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
         <v>13</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
+        <v>89</v>
+      </c>
+      <c r="D5" t="s">
         <v>14</v>
-      </c>
-      <c r="C5" t="s">
-        <v>90</v>
-      </c>
-      <c r="D5" t="s">
-        <v>15</v>
       </c>
       <c r="E5">
         <v>23</v>
@@ -814,16 +814,16 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" t="s">
         <v>14</v>
-      </c>
-      <c r="C6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" t="s">
-        <v>15</v>
       </c>
       <c r="E6">
         <v>21</v>
@@ -831,16 +831,16 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" t="s">
         <v>17</v>
       </c>
-      <c r="B7" t="s">
-        <v>18</v>
-      </c>
       <c r="C7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E7">
         <v>5</v>
@@ -848,16 +848,16 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" t="s">
         <v>20</v>
       </c>
-      <c r="B8" t="s">
-        <v>21</v>
-      </c>
       <c r="C8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E8">
         <v>20</v>
@@ -865,16 +865,16 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" t="s">
         <v>22</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" t="s">
         <v>23</v>
-      </c>
-      <c r="C9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" t="s">
-        <v>24</v>
       </c>
       <c r="E9">
         <v>18</v>
@@ -882,16 +882,16 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" t="s">
         <v>25</v>
       </c>
-      <c r="B10" t="s">
-        <v>26</v>
-      </c>
       <c r="C10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E10">
         <v>58</v>
@@ -899,16 +899,16 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" t="s">
         <v>27</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" t="s">
         <v>28</v>
-      </c>
-      <c r="C11" t="s">
-        <v>19</v>
-      </c>
-      <c r="D11" t="s">
-        <v>29</v>
       </c>
       <c r="E11">
         <v>52</v>
@@ -916,16 +916,16 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" t="s">
+        <v>90</v>
+      </c>
+      <c r="D12" t="s">
         <v>30</v>
-      </c>
-      <c r="C12" t="s">
-        <v>91</v>
-      </c>
-      <c r="D12" t="s">
-        <v>31</v>
       </c>
       <c r="E12">
         <v>17</v>
@@ -933,16 +933,16 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" t="s">
         <v>32</v>
       </c>
-      <c r="B13" t="s">
-        <v>33</v>
-      </c>
       <c r="C13" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E13">
         <v>16</v>
@@ -950,16 +950,16 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" t="s">
         <v>34</v>
       </c>
-      <c r="B14" t="s">
-        <v>35</v>
-      </c>
       <c r="C14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E14">
         <v>39</v>
@@ -967,16 +967,16 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" t="s">
         <v>36</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
+        <v>88</v>
+      </c>
+      <c r="D15" t="s">
         <v>37</v>
-      </c>
-      <c r="C15" t="s">
-        <v>89</v>
-      </c>
-      <c r="D15" t="s">
-        <v>38</v>
       </c>
       <c r="E15">
         <v>21</v>
@@ -984,16 +984,16 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" t="s">
         <v>39</v>
       </c>
-      <c r="B16" t="s">
-        <v>40</v>
-      </c>
       <c r="C16" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E16">
         <v>13</v>
@@ -1001,16 +1001,16 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B17" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" t="s">
         <v>41</v>
-      </c>
-      <c r="C17" t="s">
-        <v>8</v>
-      </c>
-      <c r="D17" t="s">
-        <v>42</v>
       </c>
       <c r="E17">
         <v>10</v>
@@ -1018,16 +1018,16 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
+        <v>42</v>
+      </c>
+      <c r="B18" t="s">
         <v>43</v>
       </c>
-      <c r="B18" t="s">
-        <v>44</v>
-      </c>
       <c r="C18" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D18" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E18">
         <v>20</v>
@@ -1035,16 +1035,16 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E19">
         <v>19</v>
@@ -1052,16 +1052,16 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B20" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C20" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D20" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E20">
         <v>9</v>
@@ -1069,16 +1069,16 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
+        <v>46</v>
+      </c>
+      <c r="B21" t="s">
         <v>47</v>
       </c>
-      <c r="B21" t="s">
-        <v>48</v>
-      </c>
       <c r="C21" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D21" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E21">
         <v>8</v>
@@ -1086,16 +1086,16 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
+        <v>48</v>
+      </c>
+      <c r="B22" t="s">
         <v>49</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
+        <v>93</v>
+      </c>
+      <c r="D22" t="s">
         <v>50</v>
-      </c>
-      <c r="C22" t="s">
-        <v>94</v>
-      </c>
-      <c r="D22" t="s">
-        <v>51</v>
       </c>
       <c r="E22">
         <v>18</v>
@@ -1103,16 +1103,16 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
+        <v>51</v>
+      </c>
+      <c r="B23" t="s">
         <v>52</v>
       </c>
-      <c r="B23" t="s">
-        <v>53</v>
-      </c>
       <c r="C23" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D23" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E23">
         <v>17</v>
@@ -1120,16 +1120,16 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
+        <v>53</v>
+      </c>
+      <c r="B24" t="s">
         <v>54</v>
       </c>
-      <c r="B24" t="s">
-        <v>55</v>
-      </c>
       <c r="C24" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D24" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E24">
         <v>6</v>
@@ -1137,16 +1137,16 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B25" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C25" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D25" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E25">
         <v>4</v>
@@ -1154,16 +1154,16 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
+        <v>56</v>
+      </c>
+      <c r="B26" t="s">
         <v>57</v>
       </c>
-      <c r="B26" t="s">
-        <v>58</v>
-      </c>
       <c r="C26" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D26" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E26">
         <v>2</v>
@@ -1171,16 +1171,16 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
+        <v>58</v>
+      </c>
+      <c r="B27" t="s">
         <v>59</v>
       </c>
-      <c r="B27" t="s">
-        <v>60</v>
-      </c>
       <c r="C27" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D27" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E27">
         <v>304</v>
@@ -1188,16 +1188,16 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B28" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C28" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D28" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E28">
         <v>254</v>
@@ -1205,16 +1205,16 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B29" t="s">
+        <v>62</v>
+      </c>
+      <c r="C29" t="s">
+        <v>7</v>
+      </c>
+      <c r="D29" t="s">
         <v>63</v>
-      </c>
-      <c r="C29" t="s">
-        <v>8</v>
-      </c>
-      <c r="D29" t="s">
-        <v>64</v>
       </c>
       <c r="E29">
         <v>151</v>
@@ -1222,16 +1222,16 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B30" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C30" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D30" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E30">
         <v>16</v>
@@ -1239,16 +1239,16 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
+        <v>65</v>
+      </c>
+      <c r="B31" t="s">
         <v>66</v>
       </c>
-      <c r="B31" t="s">
-        <v>67</v>
-      </c>
       <c r="C31" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D31" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E31">
         <v>30</v>
@@ -1256,16 +1256,16 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B32" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C32" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D32" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E32">
         <v>34</v>
@@ -1273,16 +1273,16 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
+        <v>68</v>
+      </c>
+      <c r="B33" t="s">
         <v>69</v>
       </c>
-      <c r="B33" t="s">
-        <v>70</v>
-      </c>
       <c r="C33" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D33" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E33">
         <v>13</v>
@@ -1290,16 +1290,16 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B34" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C34" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D34" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E34">
         <v>7</v>
@@ -1307,16 +1307,16 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
+        <v>71</v>
+      </c>
+      <c r="B35" t="s">
         <v>72</v>
       </c>
-      <c r="B35" t="s">
-        <v>73</v>
-      </c>
       <c r="C35" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D35" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E35">
         <v>148</v>
@@ -1324,16 +1324,16 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B36" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C36" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D36" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E36">
         <v>206</v>
@@ -1341,16 +1341,16 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
+        <v>74</v>
+      </c>
+      <c r="B37" t="s">
         <v>75</v>
       </c>
-      <c r="B37" t="s">
-        <v>76</v>
-      </c>
       <c r="C37" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D37" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E37">
         <v>40</v>
@@ -1358,16 +1358,16 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B38" t="s">
+        <v>76</v>
+      </c>
+      <c r="C38" t="s">
+        <v>7</v>
+      </c>
+      <c r="D38" t="s">
         <v>77</v>
-      </c>
-      <c r="C38" t="s">
-        <v>8</v>
-      </c>
-      <c r="D38" t="s">
-        <v>78</v>
       </c>
       <c r="E38">
         <v>63</v>
@@ -1375,16 +1375,16 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
+        <v>78</v>
+      </c>
+      <c r="B39" t="s">
         <v>79</v>
       </c>
-      <c r="B39" t="s">
-        <v>80</v>
-      </c>
       <c r="C39" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D39" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E39">
         <v>56</v>
@@ -1392,16 +1392,16 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
+        <v>80</v>
+      </c>
+      <c r="B40" t="s">
         <v>81</v>
       </c>
-      <c r="B40" t="s">
-        <v>82</v>
-      </c>
       <c r="C40" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D40" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E40">
         <v>6</v>
@@ -1409,16 +1409,16 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B41" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C41" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D41" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E41">
         <v>55</v>
@@ -1426,16 +1426,16 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B42" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C42" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D42" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E42">
         <v>43</v>
@@ -1443,16 +1443,16 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
+        <v>84</v>
+      </c>
+      <c r="B43" t="s">
         <v>85</v>
       </c>
-      <c r="B43" t="s">
-        <v>86</v>
-      </c>
       <c r="C43" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D43" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E43">
         <v>50</v>
@@ -1460,16 +1460,16 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B44" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C44" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D44" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E44">
         <v>48</v>
@@ -1477,16 +1477,16 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B45" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C45" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D45" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E45">
         <v>196</v>

</xml_diff>